<commit_message>
Changed code so it imports tickers/dates/etc from an excel file.
</commit_message>
<xml_diff>
--- a/stocks_and_dates.xlsx
+++ b/stocks_and_dates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Stock</t>
   </si>
@@ -31,7 +31,13 @@
     <t>AMZN</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>GOOGL</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>MSFT</t>
@@ -42,7 +48,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +59,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -89,17 +101,17 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -439,11 +451,13 @@
       <c r="C2" s="3">
         <v>44197</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>43831</v>
@@ -451,11 +465,13 @@
       <c r="C3" s="3">
         <v>44197</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>43831</v>
@@ -463,7 +479,9 @@
       <c r="C4" s="3">
         <v>44197</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed stocks and dates
</commit_message>
<xml_diff>
--- a/stocks_and_dates.xlsx
+++ b/stocks_and_dates.xlsx
@@ -1,66 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eth4n\Documents\Python Projects\finfluencer-finance\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D128BE-BB99-41E5-96CB-84165BC55684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="32925" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>Stock</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>Done?</t>
   </si>
   <si>
-    <t>AMZN</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>GOOGL</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>MSFT</t>
+    <t>EA Date</t>
+  </si>
+  <si>
+    <t>aapl</t>
+  </si>
+  <si>
+    <t>tsla</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -96,32 +92,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -132,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -173,71 +171,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -265,7 +263,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -288,11 +286,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -301,13 +299,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -317,7 +315,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -326,7 +324,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -335,7 +333,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -343,10 +341,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -411,76 +409,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44679</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44588</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>43831</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44197</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C4" s="6">
+        <v>44497</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>44404</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44762</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>43831</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44197</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <v>44671</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44587</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
-        <v>43831</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44197</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>44489</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>44707</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6">
+        <v>44623</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44539</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6">
+        <v>44462</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>